<commit_message>
Git sh to ease commit and push
</commit_message>
<xml_diff>
--- a/controlRoom_server/server/templates/ICR_TEMPLATE013.xlsx
+++ b/controlRoom_server/server/templates/ICR_TEMPLATE013.xlsx
@@ -3,72 +3,77 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E29A948-4A8A-8748-8933-DC71A4DC9380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2968C14-D7A6-DE4B-A1C1-142C55FEFC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICR_TEMPLATE013.xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={E018FDED-38BE-B046-9843-50C8E1BE3639}</author>
+    <author>tc={418E766E-2950-7242-BFFB-8D4643DAC7E9}</author>
+    <author>tc={3EA6EFC2-EC9E-FF44-BAC5-EF28A2989F77}</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E018FDED-38BE-B046-9843-50C8E1BE3639}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{418E766E-2950-7242-BFFB-8D4643DAC7E9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Optional.</t>
+    make sure
+ TEXT format (MM/DD/RRRR)</t>
       </text>
+    </comment>
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{3EA6EFC2-EC9E-FF44-BAC5-EF28A2989F77}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    make sure
+ TEXT format (MM/DD/RRRR)</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text/>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>SITE_CODE</t>
   </si>
   <si>
+    <t>ORDER_DATE</t>
+  </si>
+  <si>
+    <t>DELIVERY_DATE</t>
+  </si>
+  <si>
+    <t>ORDER_STATUS</t>
+  </si>
+  <si>
     <t>ITEM_CODE</t>
   </si>
   <si>
     <t>LV_CODE</t>
   </si>
   <si>
+    <t>QTY</t>
+  </si>
+  <si>
     <t>45</t>
   </si>
   <si>
-    <t>QTY</t>
-  </si>
-  <si>
-    <t>DELIVERY_DATE</t>
-  </si>
-  <si>
-    <t>ORDER_STATUS</t>
-  </si>
-  <si>
     <t>904292</t>
   </si>
   <si>
@@ -78,19 +83,13 @@
     <t>109888</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>07/13/2025</t>
-  </si>
-  <si>
-    <t>07/20/2025</t>
-  </si>
-  <si>
-    <t>ORDER_DATE</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>9/13/25</t>
+  </si>
+  <si>
+    <t>9/20/25</t>
   </si>
 </sst>
 </file>
@@ -98,11 +97,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -144,12 +150,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -205,37 +205,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -253,10 +250,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,8 +549,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F1" dT="2025-07-12T09:00:16.78" personId="{00000000-0000-0000-0000-000000000000}" id="{E018FDED-38BE-B046-9843-50C8E1BE3639}">
-    <text>Optional.</text>
+  <threadedComment ref="B1" dT="2025-07-15T14:20:12.75" personId="{00000000-0000-0000-0000-000000000000}" id="{418E766E-2950-7242-BFFB-8D4643DAC7E9}">
+    <text>make sure
+ TEXT format (MM/DD/RRRR)</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2025-07-15T14:20:21.63" personId="{00000000-0000-0000-0000-000000000000}" id="{3EA6EFC2-EC9E-FF44-BAC5-EF28A2989F77}">
+    <text>make sure
+ TEXT format (MM/DD/RRRR)</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -567,111 +565,111 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="14" width="65" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13" style="3" customWidth="1"/>
+    <col min="8" max="13" width="10.83203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="65" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
+      <c r="A2" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
+      <c r="A3" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
+      <c r="A4" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
-        <v>11</v>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{331DF5BE-6F74-5F44-80D9-83BC4620DF12}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"2,3,5"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>